<commit_message>
Final commit for implementation by openCL, SIMD and OpenMP single and four threaded
</commit_message>
<xml_diff>
--- a/project7/Workbook1.xlsx
+++ b/project7/Workbook1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2180" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Performance:931.460365</t>
   </si>
@@ -45,6 +45,12 @@
   <si>
     <t xml:space="preserve">Performance:1763.705
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenCL </t>
+  </si>
+  <si>
+    <t>OpenMP(4-threads)</t>
   </si>
 </sst>
 </file>
@@ -96,8 +102,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -131,7 +141,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -145,6 +155,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -158,6 +170,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -172,13 +186,32 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="107"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="7"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sums[*] vs Shift</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3282,37 +3315,82 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2135824008"/>
-        <c:axId val="2112427368"/>
+        <c:axId val="-2145864104"/>
+        <c:axId val="-2145767080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2135824008"/>
+        <c:axId val="-2145864104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Shift</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.461010474870315"/>
+              <c:y val="0.939481268011527"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112427368"/>
+        <c:crossAx val="-2145767080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2112427368"/>
+        <c:axId val="-2145767080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sums[*]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135824008"/>
+        <c:crossAx val="-2145864104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3341,16 +3419,45 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="107"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="7"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance vs Implementation Type</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.131603989928957"/>
+          <c:y val="0.137349397590361"/>
+          <c:w val="0.835216575524801"/>
+          <c:h val="0.714016222369794"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -3359,6 +3466,64 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00203665987780041"/>
+                  <c:y val="-0.00663789014325027"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00805331562470343"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00203665987780041"/>
+                  <c:y val="-0.00602409638554219"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$9:$C$12</c:f>
@@ -3368,13 +3533,13 @@
                   <c:v>OpenMP(single)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>OpenMP(multiple)</c:v>
+                  <c:v>OpenMP(4-threads)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>OpenCL multiple</c:v>
+                  <c:v>SIMD</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SIMD</c:v>
+                  <c:v>OpenCL </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3392,10 +3557,10 @@
                   <c:v>3170.889315</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1763.705</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>49135.1834</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1763.705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3409,21 +3574,48 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2069659512"/>
-        <c:axId val="2132648568"/>
+        <c:gapWidth val="75"/>
+        <c:overlap val="40"/>
+        <c:axId val="-2146529688"/>
+        <c:axId val="-2146526600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069659512"/>
+        <c:axId val="-2146529688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Implementation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.452205365877127"/>
+              <c:y val="0.933734939759036"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132648568"/>
+        <c:crossAx val="-2146526600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3431,25 +3623,58 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132648568"/>
+        <c:axId val="-2146526600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Performance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MegaSumsElement/Second)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069659512"/>
+        <c:crossAx val="-2146529688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.873134211074939"/>
+          <c:y val="0.0339111564367707"/>
+          <c:w val="0.0983525506358548"/>
+          <c:h val="0.0604907029693577"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3469,15 +3694,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>1384300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3504,19 +3729,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1803400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3858,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12606,8 +12831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12656,7 +12881,7 @@
     </row>
     <row r="10" spans="3:6">
       <c r="C10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>3170.8893149999999</v>
@@ -12664,18 +12889,18 @@
     </row>
     <row r="11" spans="3:6">
       <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>49135.183400000002</v>
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1763.7049999999999</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="16" customHeight="1">
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1763.7049999999999</v>
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>49135.183400000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>